<commit_message>
tried the plate detection but my PC hardware is not compatible
</commit_message>
<xml_diff>
--- a/parkingLotSystem/plate_detection/authorized_plates.xlsx
+++ b/parkingLotSystem/plate_detection/authorized_plates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,29 +436,29 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>plate</t>
+          <t>Plate_Number</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>owner_name</t>
+          <t>Owner_Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>vehicle_type</t>
+          <t>Vehicle_Type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>notes</t>
+          <t>Registration_Date</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>34ABC123</t>
+          <t>ABC 123 XYZ</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,19 +468,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Car</t>
+          <t>Sedan</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Regular visitor</t>
+          <t>2024-01-15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>06DEF456</t>
+          <t>DEF 456 UVW</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -495,29 +495,183 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Staff member</t>
+          <t>2024-02-20</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>35GHI789</t>
+          <t>GHI 789 RST</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Admin Vehicle</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Van</t>
+          <t>Truck</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Company vehicle</t>
+          <t>2024-03-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JKL 012 PQR</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Alice Williams</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sedan</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-03-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MNO 345 LMN</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Charlie Brown</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Hatchback</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2024-04-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>PQR 678 JKL</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Diana Davis</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SUV</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2024-04-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>STU 901 GHI</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Eva Wilson</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Sedan</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2024-05-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>VWX 234 DEF</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Frank Miller</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-05-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>YZA 567 ABC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Grace Taylor</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SUV</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-06-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BCD 890 ZYX</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Henry Anderson</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sedan</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2024-06-20</t>
         </is>
       </c>
     </row>

</xml_diff>